<commit_message>
xlsx <-> csv not working
works only if the ouptut of tst_csv_xlsx is opened with libreoffice and saved, then readed
if the csv is saved, empty cells (without text) lose the "" in the ||
</commit_message>
<xml_diff>
--- a/tests/files/ts_xlsx/completeIn.xlsx
+++ b/tests/files/ts_xlsx/completeIn.xlsx
@@ -1696,7 +1696,1028 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="51" min="51" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="52" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="55" min="55" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="56" min="56" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="57" min="57" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="58" min="58" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="59" min="59" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="60" min="60" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="61" min="61" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="62" min="62" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="63" min="63" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="64" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="65" min="65" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="66" min="66" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="67" min="67" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="68" min="68" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="69" min="69" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="70" min="70" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="71" min="71" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="72" min="72" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="73" min="73" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="74" min="74" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="75" min="75" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="76" min="76" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="77" min="77" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="78" min="78" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="79" min="79" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="80" min="80" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="81" min="81" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="82" min="82" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="83" min="83" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="84" min="84" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="85" min="85" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="86" min="86" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="87" min="87" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="88" min="88" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="89" min="89" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="90" min="90" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="91" min="91" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="92" min="92" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="93" min="93" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="94" min="94" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="95" min="95" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="96" min="96" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="97" min="97" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="98" min="98" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="99" min="99" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="100" min="100" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="101" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="102" min="102" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="103" min="103" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="104" min="104" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="105" min="105" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="106" min="106" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="107" min="107" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="108" min="108" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="109" min="109" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="110" min="110" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="111" min="111" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="112" min="112" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="113" min="113" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="114" min="114" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="115" min="115" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="116" min="116" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="117" min="117" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="118" min="118" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="119" min="119" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="120" min="120" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="121" min="121" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="122" min="122" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="123" min="123" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="124" min="124" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="125" min="125" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="126" min="126" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="127" min="127" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="128" min="128" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="129" min="129" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="130" min="130" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="131" min="131" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="132" min="132" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="133" min="133" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="134" min="134" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="135" min="135" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="136" min="136" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="137" min="137" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="138" min="138" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="139" min="139" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="140" min="140" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="141" min="141" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="142" min="142" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="143" min="143" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="144" min="144" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="145" min="145" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="146" min="146" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="147" min="147" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="148" min="148" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="149" min="149" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="150" min="150" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="151" min="151" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="152" min="152" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="153" min="153" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="154" min="154" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="155" min="155" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="156" min="156" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="157" min="157" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="158" min="158" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="159" min="159" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="160" min="160" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="161" min="161" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="162" min="162" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="163" min="163" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="164" min="164" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="165" min="165" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="166" min="166" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="167" min="167" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="168" min="168" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="169" min="169" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="170" min="170" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="171" min="171" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="172" min="172" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="173" min="173" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="174" min="174" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="175" min="175" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="176" min="176" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="177" min="177" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="178" min="178" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="179" min="179" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="180" min="180" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="181" min="181" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="182" min="182" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="183" min="183" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="184" min="184" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="185" min="185" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="186" min="186" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="187" min="187" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="188" min="188" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="189" min="189" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="190" min="190" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="191" min="191" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="192" min="192" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="193" min="193" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="194" min="194" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="195" min="195" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="196" min="196" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="197" min="197" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="198" min="198" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="199" min="199" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="200" min="200" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="201" min="201" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="202" min="202" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="203" min="203" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="204" min="204" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="205" min="205" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="206" min="206" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="207" min="207" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="208" min="208" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="209" min="209" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="210" min="210" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="211" min="211" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="212" min="212" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="213" min="213" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="214" min="214" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="215" min="215" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="216" min="216" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="217" min="217" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="218" min="218" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="219" min="219" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="220" min="220" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="221" min="221" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="222" min="222" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="223" min="223" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="224" min="224" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="225" min="225" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="226" min="226" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="227" min="227" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="228" min="228" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="229" min="229" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="230" min="230" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="231" min="231" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="232" min="232" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="233" min="233" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="234" min="234" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="235" min="235" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="236" min="236" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="237" min="237" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="238" min="238" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="239" min="239" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="240" min="240" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="241" min="241" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="242" min="242" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="243" min="243" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="244" min="244" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="245" min="245" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="246" min="246" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="247" min="247" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="248" min="248" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="249" min="249" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="250" min="250" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="251" min="251" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="252" min="252" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="253" min="253" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="254" min="254" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="255" min="255" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="256" min="256" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="257" min="257" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="258" min="258" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="259" min="259" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="260" min="260" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="261" min="261" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="262" min="262" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="263" min="263" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="264" min="264" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="265" min="265" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="266" min="266" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="267" min="267" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="268" min="268" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="269" min="269" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="270" min="270" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="271" min="271" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="272" min="272" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="273" min="273" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="274" min="274" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="275" min="275" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="276" min="276" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="277" min="277" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="278" min="278" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="279" min="279" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="280" min="280" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="281" min="281" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="282" min="282" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="283" min="283" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="284" min="284" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="285" min="285" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="286" min="286" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="287" min="287" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="288" min="288" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="289" min="289" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="290" min="290" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="291" min="291" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="292" min="292" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="293" min="293" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="294" min="294" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="295" min="295" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="296" min="296" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="297" min="297" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="298" min="298" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="299" min="299" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="300" min="300" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="301" min="301" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="302" min="302" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="303" min="303" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="304" min="304" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="305" min="305" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="306" min="306" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="307" min="307" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="308" min="308" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="309" min="309" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="310" min="310" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="311" min="311" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="312" min="312" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="313" min="313" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="314" min="314" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="315" min="315" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="316" min="316" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="317" min="317" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="318" min="318" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="319" min="319" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="320" min="320" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="321" min="321" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="322" min="322" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="323" min="323" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="324" min="324" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="325" min="325" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="326" min="326" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="327" min="327" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="328" min="328" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="329" min="329" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="330" min="330" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="331" min="331" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="332" min="332" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="333" min="333" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="334" min="334" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="335" min="335" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="336" min="336" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="337" min="337" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="338" min="338" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="339" min="339" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="340" min="340" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="341" min="341" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="342" min="342" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="343" min="343" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="344" min="344" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="345" min="345" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="346" min="346" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="347" min="347" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="348" min="348" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="349" min="349" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="350" min="350" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="351" min="351" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="352" min="352" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="353" min="353" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="354" min="354" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="355" min="355" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="356" min="356" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="357" min="357" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="358" min="358" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="359" min="359" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="360" min="360" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="361" min="361" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="362" min="362" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="363" min="363" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="364" min="364" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="365" min="365" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="366" min="366" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="367" min="367" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="368" min="368" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="369" min="369" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="370" min="370" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="371" min="371" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="372" min="372" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="373" min="373" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="374" min="374" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="375" min="375" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="376" min="376" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="377" min="377" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="378" min="378" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="379" min="379" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="380" min="380" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="381" min="381" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="382" min="382" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="383" min="383" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="384" min="384" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="385" min="385" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="386" min="386" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="387" min="387" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="388" min="388" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="389" min="389" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="390" min="390" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="391" min="391" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="392" min="392" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="393" min="393" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="394" min="394" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="395" min="395" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="396" min="396" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="397" min="397" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="398" min="398" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="399" min="399" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="400" min="400" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="401" min="401" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="402" min="402" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="403" min="403" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="404" min="404" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="405" min="405" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="406" min="406" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="407" min="407" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="408" min="408" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="409" min="409" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="410" min="410" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="411" min="411" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="412" min="412" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="413" min="413" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="414" min="414" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="415" min="415" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="416" min="416" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="417" min="417" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="418" min="418" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="419" min="419" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="420" min="420" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="421" min="421" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="422" min="422" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="423" min="423" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="424" min="424" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="425" min="425" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="426" min="426" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="427" min="427" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="428" min="428" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="429" min="429" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="430" min="430" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="431" min="431" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="432" min="432" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="433" min="433" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="434" min="434" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="435" min="435" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="436" min="436" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="437" min="437" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="438" min="438" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="439" min="439" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="440" min="440" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="441" min="441" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="442" min="442" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="443" min="443" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="444" min="444" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="445" min="445" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="446" min="446" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="447" min="447" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="448" min="448" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="449" min="449" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="450" min="450" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="451" min="451" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="452" min="452" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="453" min="453" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="454" min="454" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="455" min="455" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="456" min="456" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="457" min="457" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="458" min="458" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="459" min="459" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="460" min="460" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="461" min="461" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="462" min="462" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="463" min="463" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="464" min="464" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="465" min="465" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="466" min="466" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="467" min="467" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="468" min="468" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="469" min="469" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="470" min="470" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="471" min="471" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="472" min="472" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="473" min="473" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="474" min="474" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="475" min="475" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="476" min="476" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="477" min="477" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="478" min="478" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="479" min="479" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="480" min="480" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="481" min="481" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="482" min="482" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="483" min="483" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="484" min="484" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="485" min="485" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="486" min="486" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="487" min="487" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="488" min="488" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="489" min="489" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="490" min="490" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="491" min="491" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="492" min="492" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="493" min="493" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="494" min="494" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="495" min="495" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="496" min="496" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="497" min="497" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="498" min="498" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="499" min="499" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="500" min="500" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="501" min="501" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="502" min="502" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="503" min="503" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="504" min="504" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="505" min="505" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="506" min="506" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="507" min="507" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="508" min="508" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="509" min="509" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="510" min="510" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="511" min="511" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="512" min="512" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="513" min="513" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="514" min="514" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="515" min="515" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="516" min="516" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="517" min="517" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="518" min="518" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="519" min="519" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="520" min="520" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="521" min="521" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="522" min="522" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="523" min="523" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="524" min="524" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="525" min="525" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="526" min="526" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="527" min="527" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="528" min="528" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="529" min="529" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="530" min="530" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="531" min="531" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="532" min="532" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="533" min="533" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="534" min="534" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="535" min="535" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="536" min="536" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="537" min="537" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="538" min="538" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="539" min="539" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="540" min="540" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="541" min="541" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="542" min="542" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="543" min="543" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="544" min="544" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="545" min="545" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="546" min="546" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="547" min="547" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="548" min="548" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="549" min="549" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="550" min="550" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="551" min="551" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="552" min="552" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="553" min="553" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="554" min="554" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="555" min="555" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="556" min="556" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="557" min="557" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="558" min="558" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="559" min="559" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="560" min="560" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="561" min="561" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="562" min="562" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="563" min="563" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="564" min="564" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="565" min="565" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="566" min="566" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="567" min="567" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="568" min="568" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="569" min="569" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="570" min="570" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="571" min="571" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="572" min="572" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="573" min="573" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="574" min="574" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="575" min="575" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="576" min="576" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="577" min="577" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="578" min="578" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="579" min="579" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="580" min="580" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="581" min="581" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="582" min="582" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="583" min="583" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="584" min="584" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="585" min="585" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="586" min="586" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="587" min="587" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="588" min="588" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="589" min="589" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="590" min="590" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="591" min="591" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="592" min="592" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="593" min="593" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="594" min="594" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="595" min="595" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="596" min="596" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="597" min="597" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="598" min="598" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="599" min="599" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="600" min="600" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="601" min="601" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="602" min="602" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="603" min="603" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="604" min="604" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="605" min="605" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="606" min="606" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="607" min="607" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="608" min="608" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="609" min="609" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="610" min="610" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="611" min="611" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="612" min="612" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="613" min="613" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="614" min="614" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="615" min="615" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="616" min="616" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="617" min="617" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="618" min="618" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="619" min="619" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="620" min="620" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="621" min="621" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="622" min="622" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="623" min="623" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="624" min="624" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="625" min="625" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="626" min="626" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="627" min="627" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="628" min="628" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="629" min="629" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="630" min="630" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="631" min="631" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="632" min="632" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="633" min="633" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="634" min="634" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="635" min="635" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="636" min="636" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="637" min="637" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="638" min="638" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="639" min="639" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="640" min="640" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="641" min="641" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="642" min="642" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="643" min="643" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="644" min="644" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="645" min="645" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="646" min="646" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="647" min="647" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="648" min="648" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="649" min="649" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="650" min="650" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="651" min="651" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="652" min="652" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="653" min="653" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="654" min="654" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="655" min="655" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="656" min="656" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="657" min="657" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="658" min="658" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="659" min="659" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="660" min="660" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="661" min="661" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="662" min="662" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="663" min="663" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="664" min="664" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="665" min="665" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="666" min="666" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="667" min="667" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="668" min="668" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="669" min="669" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="670" min="670" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="671" min="671" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="672" min="672" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="673" min="673" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="674" min="674" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="675" min="675" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="676" min="676" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="677" min="677" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="678" min="678" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="679" min="679" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="680" min="680" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="681" min="681" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="682" min="682" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="683" min="683" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="684" min="684" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="685" min="685" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="686" min="686" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="687" min="687" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="688" min="688" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="689" min="689" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="690" min="690" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="691" min="691" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="692" min="692" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="693" min="693" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="694" min="694" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="695" min="695" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="696" min="696" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="697" min="697" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="698" min="698" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="699" min="699" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="700" min="700" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="701" min="701" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="702" min="702" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="703" min="703" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="704" min="704" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="705" min="705" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="706" min="706" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="707" min="707" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="708" min="708" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="709" min="709" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="710" min="710" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="711" min="711" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="712" min="712" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="713" min="713" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="714" min="714" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="715" min="715" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="716" min="716" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="717" min="717" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="718" min="718" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="719" min="719" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="720" min="720" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="721" min="721" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="722" min="722" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="723" min="723" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="724" min="724" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="725" min="725" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="726" min="726" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="727" min="727" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="728" min="728" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="729" min="729" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="730" min="730" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="731" min="731" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="732" min="732" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="733" min="733" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="734" min="734" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="735" min="735" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="736" min="736" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="737" min="737" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="738" min="738" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="739" min="739" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="740" min="740" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="741" min="741" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="742" min="742" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="743" min="743" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="744" min="744" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="745" min="745" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="746" min="746" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="747" min="747" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="748" min="748" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="749" min="749" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="750" min="750" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="751" min="751" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="752" min="752" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="753" min="753" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="754" min="754" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="755" min="755" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="756" min="756" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="757" min="757" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="758" min="758" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="759" min="759" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="760" min="760" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="761" min="761" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="762" min="762" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="763" min="763" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="764" min="764" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="765" min="765" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="766" min="766" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="767" min="767" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="768" min="768" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="769" min="769" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="770" min="770" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="771" min="771" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="772" min="772" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="773" min="773" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="774" min="774" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="775" min="775" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="776" min="776" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="777" min="777" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="778" min="778" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="779" min="779" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="780" min="780" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="781" min="781" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="782" min="782" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="783" min="783" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="784" min="784" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="785" min="785" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="786" min="786" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="787" min="787" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="788" min="788" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="789" min="789" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="790" min="790" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="791" min="791" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="792" min="792" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="793" min="793" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="794" min="794" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="795" min="795" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="796" min="796" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="797" min="797" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="798" min="798" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="799" min="799" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="800" min="800" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="801" min="801" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="802" min="802" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="803" min="803" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="804" min="804" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="805" min="805" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="806" min="806" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="807" min="807" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="808" min="808" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="809" min="809" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="810" min="810" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="811" min="811" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="812" min="812" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="813" min="813" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="814" min="814" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="815" min="815" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="816" min="816" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="817" min="817" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="818" min="818" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="819" min="819" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="820" min="820" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="821" min="821" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="822" min="822" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="823" min="823" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="824" min="824" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="825" min="825" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="826" min="826" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="827" min="827" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="828" min="828" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="829" min="829" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="830" min="830" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="831" min="831" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="832" min="832" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="833" min="833" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="834" min="834" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="835" min="835" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="836" min="836" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="837" min="837" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="838" min="838" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="839" min="839" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="840" min="840" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="841" min="841" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="842" min="842" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="843" min="843" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="844" min="844" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="845" min="845" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="846" min="846" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="847" min="847" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="848" min="848" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="849" min="849" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="850" min="850" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="851" min="851" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="852" min="852" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="853" min="853" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="854" min="854" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="855" min="855" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="856" min="856" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="857" min="857" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="858" min="858" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="859" min="859" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="860" min="860" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="861" min="861" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="862" min="862" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="863" min="863" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="864" min="864" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="865" min="865" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="866" min="866" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="867" min="867" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="868" min="868" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="869" min="869" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="870" min="870" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="871" min="871" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="872" min="872" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="873" min="873" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="874" min="874" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="875" min="875" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="876" min="876" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="877" min="877" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="878" min="878" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="879" min="879" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="880" min="880" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="881" min="881" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="882" min="882" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="883" min="883" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="884" min="884" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="885" min="885" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="886" min="886" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="887" min="887" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="888" min="888" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="889" min="889" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="890" min="890" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="891" min="891" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="892" min="892" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="893" min="893" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="894" min="894" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="895" min="895" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="896" min="896" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="897" min="897" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="898" min="898" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="899" min="899" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="900" min="900" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="901" min="901" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="902" min="902" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="903" min="903" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="904" min="904" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="905" min="905" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="906" min="906" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="907" min="907" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="908" min="908" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="909" min="909" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="910" min="910" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="911" min="911" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="912" min="912" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="913" min="913" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="914" min="914" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="915" min="915" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="916" min="916" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="917" min="917" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="918" min="918" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="919" min="919" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="920" min="920" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="921" min="921" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="922" min="922" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="923" min="923" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="924" min="924" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="925" min="925" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="926" min="926" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="927" min="927" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="928" min="928" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="929" min="929" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="930" min="930" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="931" min="931" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="932" min="932" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="933" min="933" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="934" min="934" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="935" min="935" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="936" min="936" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="937" min="937" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="938" min="938" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="939" min="939" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="940" min="940" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="941" min="941" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="942" min="942" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="943" min="943" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="944" min="944" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="945" min="945" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="946" min="946" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="947" min="947" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="948" min="948" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="949" min="949" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="950" min="950" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="951" min="951" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="952" min="952" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="953" min="953" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="954" min="954" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="955" min="955" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="956" min="956" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="957" min="957" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="958" min="958" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="959" min="959" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="960" min="960" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="961" min="961" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="962" min="962" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="963" min="963" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="964" min="964" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="965" min="965" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="966" min="966" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="967" min="967" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="968" min="968" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="969" min="969" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="970" min="970" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="971" min="971" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="972" min="972" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="973" min="973" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="974" min="974" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="975" min="975" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="976" min="976" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="977" min="977" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="978" min="978" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="979" min="979" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="980" min="980" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="981" min="981" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="982" min="982" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="983" min="983" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="984" min="984" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="985" min="985" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="986" min="986" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="987" min="987" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="988" min="988" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="989" min="989" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="990" min="990" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="991" min="991" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="992" min="992" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="993" min="993" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="994" min="994" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="995" min="995" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="996" min="996" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="997" min="997" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="998" min="998" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="999" min="999" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1000" min="1000" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1001" min="1001" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1002" min="1002" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1003" min="1003" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1004" min="1004" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1005" min="1005" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1006" min="1006" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1007" min="1007" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1008" min="1008" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1009" min="1009" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1010" min="1010" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1011" min="1011" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1012" min="1012" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1013" min="1013" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1014" min="1014" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1015" min="1015" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1016" min="1016" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1017" min="1017" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1018" min="1018" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1019" min="1019" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1020" min="1020" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1021" min="1021" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="1022" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="1023" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1025" style="0" width="8.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1735,6 +2756,7 @@
       <c r="D2" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="E2"/>
       <c r="F2" s="0" t="s">
         <v>10</v>
       </c>
@@ -1755,6 +2777,9 @@
       <c r="D3" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="E3"/>
+      <c r="F3"/>
+      <c r="G3"/>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
@@ -1769,6 +2794,9 @@
       <c r="D4" s="0" t="s">
         <v>15</v>
       </c>
+      <c r="E4"/>
+      <c r="F4"/>
+      <c r="G4"/>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
@@ -1783,6 +2811,9 @@
       <c r="D5" s="0" t="s">
         <v>15</v>
       </c>
+      <c r="E5"/>
+      <c r="F5"/>
+      <c r="G5"/>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
@@ -1797,6 +2828,9 @@
       <c r="D6" s="0" t="s">
         <v>20</v>
       </c>
+      <c r="E6"/>
+      <c r="F6"/>
+      <c r="G6"/>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
@@ -1811,6 +2845,9 @@
       <c r="D7" s="0" t="s">
         <v>23</v>
       </c>
+      <c r="E7"/>
+      <c r="F7"/>
+      <c r="G7"/>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
@@ -1825,6 +2862,9 @@
       <c r="D8" s="0" t="s">
         <v>26</v>
       </c>
+      <c r="E8"/>
+      <c r="F8"/>
+      <c r="G8"/>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
@@ -1839,6 +2879,9 @@
       <c r="D9" s="0" t="s">
         <v>29</v>
       </c>
+      <c r="E9"/>
+      <c r="F9"/>
+      <c r="G9"/>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
@@ -1853,6 +2896,9 @@
       <c r="D10" s="0" t="s">
         <v>20</v>
       </c>
+      <c r="E10"/>
+      <c r="F10"/>
+      <c r="G10"/>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
@@ -1867,6 +2913,9 @@
       <c r="D11" s="0" t="s">
         <v>33</v>
       </c>
+      <c r="E11"/>
+      <c r="F11"/>
+      <c r="G11"/>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
@@ -1881,6 +2930,9 @@
       <c r="D12" s="0" t="s">
         <v>33</v>
       </c>
+      <c r="E12"/>
+      <c r="F12"/>
+      <c r="G12"/>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
@@ -1898,6 +2950,8 @@
       <c r="E13" s="0" t="s">
         <v>39</v>
       </c>
+      <c r="F13"/>
+      <c r="G13"/>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
@@ -1912,6 +2966,9 @@
       <c r="D14" s="0" t="s">
         <v>43</v>
       </c>
+      <c r="E14"/>
+      <c r="F14"/>
+      <c r="G14"/>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
@@ -1926,6 +2983,9 @@
       <c r="D15" s="0" t="s">
         <v>46</v>
       </c>
+      <c r="E15"/>
+      <c r="F15"/>
+      <c r="G15"/>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
@@ -1943,6 +3003,8 @@
       <c r="E16" s="0" t="s">
         <v>49</v>
       </c>
+      <c r="F16"/>
+      <c r="G16"/>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
@@ -1957,6 +3019,9 @@
       <c r="D17" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="E17"/>
+      <c r="F17"/>
+      <c r="G17"/>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
@@ -1971,6 +3036,9 @@
       <c r="D18" s="0" t="s">
         <v>56</v>
       </c>
+      <c r="E18"/>
+      <c r="F18"/>
+      <c r="G18"/>
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
@@ -1985,6 +3053,9 @@
       <c r="D19" s="0" t="s">
         <v>58</v>
       </c>
+      <c r="E19"/>
+      <c r="F19"/>
+      <c r="G19"/>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
@@ -1999,6 +3070,9 @@
       <c r="D20" s="0" t="s">
         <v>62</v>
       </c>
+      <c r="E20"/>
+      <c r="F20"/>
+      <c r="G20"/>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
@@ -2013,6 +3087,9 @@
       <c r="D21" s="0" t="s">
         <v>65</v>
       </c>
+      <c r="E21"/>
+      <c r="F21"/>
+      <c r="G21"/>
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
@@ -2027,6 +3104,9 @@
       <c r="D22" s="0" t="s">
         <v>68</v>
       </c>
+      <c r="E22"/>
+      <c r="F22"/>
+      <c r="G22"/>
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
@@ -2041,6 +3121,9 @@
       <c r="D23" s="0" t="s">
         <v>71</v>
       </c>
+      <c r="E23"/>
+      <c r="F23"/>
+      <c r="G23"/>
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
@@ -2055,6 +3138,9 @@
       <c r="D24" s="0" t="s">
         <v>72</v>
       </c>
+      <c r="E24"/>
+      <c r="F24"/>
+      <c r="G24"/>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
@@ -2069,6 +3155,9 @@
       <c r="D25" s="0" t="s">
         <v>74</v>
       </c>
+      <c r="E25"/>
+      <c r="F25"/>
+      <c r="G25"/>
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
@@ -2083,6 +3172,9 @@
       <c r="D26" s="0" t="s">
         <v>78</v>
       </c>
+      <c r="E26"/>
+      <c r="F26"/>
+      <c r="G26"/>
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
@@ -2097,6 +3189,9 @@
       <c r="D27" s="0" t="s">
         <v>82</v>
       </c>
+      <c r="E27"/>
+      <c r="F27"/>
+      <c r="G27"/>
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
@@ -2111,6 +3206,9 @@
       <c r="D28" s="0" t="s">
         <v>83</v>
       </c>
+      <c r="E28"/>
+      <c r="F28"/>
+      <c r="G28"/>
     </row>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
@@ -2125,6 +3223,9 @@
       <c r="D29" s="0" t="s">
         <v>85</v>
       </c>
+      <c r="E29"/>
+      <c r="F29"/>
+      <c r="G29"/>
     </row>
     <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
@@ -2139,6 +3240,9 @@
       <c r="D30" s="0" t="s">
         <v>87</v>
       </c>
+      <c r="E30"/>
+      <c r="F30"/>
+      <c r="G30"/>
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
@@ -2153,6 +3257,9 @@
       <c r="D31" s="0" t="s">
         <v>90</v>
       </c>
+      <c r="E31"/>
+      <c r="F31"/>
+      <c r="G31"/>
     </row>
     <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
@@ -2170,6 +3277,8 @@
       <c r="E32" s="0" t="s">
         <v>92</v>
       </c>
+      <c r="F32"/>
+      <c r="G32"/>
     </row>
     <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
@@ -2184,6 +3293,9 @@
       <c r="D33" s="0" t="s">
         <v>94</v>
       </c>
+      <c r="E33"/>
+      <c r="F33"/>
+      <c r="G33"/>
     </row>
     <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
@@ -2198,6 +3310,9 @@
       <c r="D34" s="0" t="s">
         <v>95</v>
       </c>
+      <c r="E34"/>
+      <c r="F34"/>
+      <c r="G34"/>
     </row>
     <row r="35" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
@@ -2212,6 +3327,9 @@
       <c r="D35" s="0" t="s">
         <v>99</v>
       </c>
+      <c r="E35"/>
+      <c r="F35"/>
+      <c r="G35"/>
     </row>
     <row r="36" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
@@ -2226,6 +3344,9 @@
       <c r="D36" s="0" t="s">
         <v>103</v>
       </c>
+      <c r="E36"/>
+      <c r="F36"/>
+      <c r="G36"/>
     </row>
     <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
@@ -2240,6 +3361,9 @@
       <c r="D37" s="0" t="s">
         <v>105</v>
       </c>
+      <c r="E37"/>
+      <c r="F37"/>
+      <c r="G37"/>
     </row>
     <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
@@ -2254,6 +3378,9 @@
       <c r="D38" s="0" t="s">
         <v>105</v>
       </c>
+      <c r="E38"/>
+      <c r="F38"/>
+      <c r="G38"/>
     </row>
     <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
@@ -2268,6 +3395,9 @@
       <c r="D39" s="0" t="s">
         <v>111</v>
       </c>
+      <c r="E39"/>
+      <c r="F39"/>
+      <c r="G39"/>
     </row>
     <row r="40" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
@@ -2282,6 +3412,9 @@
       <c r="D40" s="0" t="s">
         <v>115</v>
       </c>
+      <c r="E40"/>
+      <c r="F40"/>
+      <c r="G40"/>
     </row>
     <row r="41" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
@@ -2296,6 +3429,9 @@
       <c r="D41" s="0" t="s">
         <v>118</v>
       </c>
+      <c r="E41"/>
+      <c r="F41"/>
+      <c r="G41"/>
     </row>
     <row r="42" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
@@ -2310,6 +3446,9 @@
       <c r="D42" s="0" t="s">
         <v>121</v>
       </c>
+      <c r="E42"/>
+      <c r="F42"/>
+      <c r="G42"/>
     </row>
     <row r="43" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
@@ -2324,6 +3463,9 @@
       <c r="D43" s="0" t="s">
         <v>124</v>
       </c>
+      <c r="E43"/>
+      <c r="F43"/>
+      <c r="G43"/>
     </row>
     <row r="44" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
@@ -2338,6 +3480,9 @@
       <c r="D44" s="0" t="s">
         <v>127</v>
       </c>
+      <c r="E44"/>
+      <c r="F44"/>
+      <c r="G44"/>
     </row>
     <row r="45" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
@@ -2352,6 +3497,9 @@
       <c r="D45" s="0" t="s">
         <v>130</v>
       </c>
+      <c r="E45"/>
+      <c r="F45"/>
+      <c r="G45"/>
     </row>
     <row r="46" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
@@ -2366,6 +3514,9 @@
       <c r="D46" s="0" t="s">
         <v>134</v>
       </c>
+      <c r="E46"/>
+      <c r="F46"/>
+      <c r="G46"/>
     </row>
     <row r="47" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
@@ -2380,6 +3531,9 @@
       <c r="D47" s="0" t="s">
         <v>138</v>
       </c>
+      <c r="E47"/>
+      <c r="F47"/>
+      <c r="G47"/>
     </row>
     <row r="48" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
@@ -2394,6 +3548,9 @@
       <c r="D48" s="0" t="s">
         <v>140</v>
       </c>
+      <c r="E48"/>
+      <c r="F48"/>
+      <c r="G48"/>
     </row>
     <row r="49" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
@@ -2408,6 +3565,9 @@
       <c r="D49" s="0" t="s">
         <v>143</v>
       </c>
+      <c r="E49"/>
+      <c r="F49"/>
+      <c r="G49"/>
     </row>
     <row r="50" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
@@ -2422,6 +3582,9 @@
       <c r="D50" s="0" t="s">
         <v>146</v>
       </c>
+      <c r="E50"/>
+      <c r="F50"/>
+      <c r="G50"/>
     </row>
     <row r="51" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
@@ -2436,6 +3599,9 @@
       <c r="D51" s="0" t="s">
         <v>149</v>
       </c>
+      <c r="E51"/>
+      <c r="F51"/>
+      <c r="G51"/>
     </row>
     <row r="52" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
@@ -2450,6 +3616,9 @@
       <c r="D52" s="0" t="s">
         <v>152</v>
       </c>
+      <c r="E52"/>
+      <c r="F52"/>
+      <c r="G52"/>
     </row>
     <row r="53" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
@@ -2464,6 +3633,9 @@
       <c r="D53" s="0" t="s">
         <v>155</v>
       </c>
+      <c r="E53"/>
+      <c r="F53"/>
+      <c r="G53"/>
     </row>
     <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
@@ -2478,6 +3650,9 @@
       <c r="D54" s="0" t="s">
         <v>158</v>
       </c>
+      <c r="E54"/>
+      <c r="F54"/>
+      <c r="G54"/>
     </row>
     <row r="55" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
@@ -2492,6 +3667,9 @@
       <c r="D55" s="0" t="s">
         <v>161</v>
       </c>
+      <c r="E55"/>
+      <c r="F55"/>
+      <c r="G55"/>
     </row>
     <row r="56" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
@@ -2506,6 +3684,9 @@
       <c r="D56" s="0" t="s">
         <v>164</v>
       </c>
+      <c r="E56"/>
+      <c r="F56"/>
+      <c r="G56"/>
     </row>
     <row r="57" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
@@ -2520,6 +3701,9 @@
       <c r="D57" s="0" t="s">
         <v>167</v>
       </c>
+      <c r="E57"/>
+      <c r="F57"/>
+      <c r="G57"/>
     </row>
     <row r="58" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
@@ -2534,6 +3718,9 @@
       <c r="D58" s="0" t="s">
         <v>170</v>
       </c>
+      <c r="E58"/>
+      <c r="F58"/>
+      <c r="G58"/>
     </row>
     <row r="59" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
@@ -2548,6 +3735,9 @@
       <c r="D59" s="0" t="s">
         <v>173</v>
       </c>
+      <c r="E59"/>
+      <c r="F59"/>
+      <c r="G59"/>
     </row>
     <row r="60" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
@@ -2565,6 +3755,8 @@
       <c r="E60" s="0" t="s">
         <v>177</v>
       </c>
+      <c r="F60"/>
+      <c r="G60"/>
     </row>
     <row r="61" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
@@ -2579,6 +3771,9 @@
       <c r="D61" s="0" t="s">
         <v>180</v>
       </c>
+      <c r="E61"/>
+      <c r="F61"/>
+      <c r="G61"/>
     </row>
     <row r="62" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
@@ -2593,6 +3788,9 @@
       <c r="D62" s="0" t="s">
         <v>184</v>
       </c>
+      <c r="E62"/>
+      <c r="F62"/>
+      <c r="G62"/>
     </row>
     <row r="63" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
@@ -2607,6 +3805,9 @@
       <c r="D63" s="0" t="s">
         <v>184</v>
       </c>
+      <c r="E63"/>
+      <c r="F63"/>
+      <c r="G63"/>
     </row>
     <row r="64" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
@@ -2621,6 +3822,9 @@
       <c r="D64" s="0" t="s">
         <v>184</v>
       </c>
+      <c r="E64"/>
+      <c r="F64"/>
+      <c r="G64"/>
     </row>
     <row r="65" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
@@ -2635,6 +3839,9 @@
       <c r="D65" s="0" t="s">
         <v>184</v>
       </c>
+      <c r="E65"/>
+      <c r="F65"/>
+      <c r="G65"/>
     </row>
     <row r="66" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
@@ -2649,6 +3856,9 @@
       <c r="D66" s="0" t="s">
         <v>184</v>
       </c>
+      <c r="E66"/>
+      <c r="F66"/>
+      <c r="G66"/>
     </row>
     <row r="67" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
@@ -2663,6 +3873,9 @@
       <c r="D67" s="0" t="s">
         <v>184</v>
       </c>
+      <c r="E67"/>
+      <c r="F67"/>
+      <c r="G67"/>
     </row>
     <row r="68" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
@@ -2677,6 +3890,9 @@
       <c r="D68" s="0" t="s">
         <v>184</v>
       </c>
+      <c r="E68"/>
+      <c r="F68"/>
+      <c r="G68"/>
     </row>
     <row r="69" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
@@ -2691,6 +3907,9 @@
       <c r="D69" s="0" t="s">
         <v>200</v>
       </c>
+      <c r="E69"/>
+      <c r="F69"/>
+      <c r="G69"/>
     </row>
     <row r="70" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
@@ -2705,6 +3924,9 @@
       <c r="D70" s="0" t="s">
         <v>202</v>
       </c>
+      <c r="E70"/>
+      <c r="F70"/>
+      <c r="G70"/>
     </row>
     <row r="71" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
@@ -2719,6 +3941,9 @@
       <c r="D71" s="0" t="s">
         <v>205</v>
       </c>
+      <c r="E71"/>
+      <c r="F71"/>
+      <c r="G71"/>
     </row>
     <row r="72" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
@@ -2733,6 +3958,9 @@
       <c r="D72" s="0" t="s">
         <v>208</v>
       </c>
+      <c r="E72"/>
+      <c r="F72"/>
+      <c r="G72"/>
     </row>
     <row r="73" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
@@ -2747,6 +3975,9 @@
       <c r="D73" s="0" t="s">
         <v>209</v>
       </c>
+      <c r="E73"/>
+      <c r="F73"/>
+      <c r="G73"/>
     </row>
     <row r="74" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
@@ -2761,6 +3992,9 @@
       <c r="D74" s="0" t="s">
         <v>209</v>
       </c>
+      <c r="E74"/>
+      <c r="F74"/>
+      <c r="G74"/>
     </row>
     <row r="75" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
@@ -2775,6 +4009,9 @@
       <c r="D75" s="0" t="s">
         <v>209</v>
       </c>
+      <c r="E75"/>
+      <c r="F75"/>
+      <c r="G75"/>
     </row>
     <row r="76" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
@@ -2789,6 +4026,9 @@
       <c r="D76" s="0" t="s">
         <v>209</v>
       </c>
+      <c r="E76"/>
+      <c r="F76"/>
+      <c r="G76"/>
     </row>
     <row r="77" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
@@ -2803,6 +4043,9 @@
       <c r="D77" s="0" t="s">
         <v>209</v>
       </c>
+      <c r="E77"/>
+      <c r="F77"/>
+      <c r="G77"/>
     </row>
     <row r="78" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
@@ -2817,6 +4060,9 @@
       <c r="D78" s="0" t="s">
         <v>209</v>
       </c>
+      <c r="E78"/>
+      <c r="F78"/>
+      <c r="G78"/>
     </row>
     <row r="79" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
@@ -2831,6 +4077,9 @@
       <c r="D79" s="0" t="s">
         <v>209</v>
       </c>
+      <c r="E79"/>
+      <c r="F79"/>
+      <c r="G79"/>
     </row>
     <row r="80" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
@@ -2845,6 +4094,9 @@
       <c r="D80" s="0" t="s">
         <v>212</v>
       </c>
+      <c r="E80"/>
+      <c r="F80"/>
+      <c r="G80"/>
     </row>
     <row r="81" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
@@ -2859,6 +4111,9 @@
       <c r="D81" s="0" t="s">
         <v>215</v>
       </c>
+      <c r="E81"/>
+      <c r="F81"/>
+      <c r="G81"/>
     </row>
     <row r="82" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
@@ -2873,6 +4128,9 @@
       <c r="D82" s="0" t="s">
         <v>219</v>
       </c>
+      <c r="E82"/>
+      <c r="F82"/>
+      <c r="G82"/>
     </row>
     <row r="83" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
@@ -2887,6 +4145,9 @@
       <c r="D83" s="0" t="s">
         <v>222</v>
       </c>
+      <c r="E83"/>
+      <c r="F83"/>
+      <c r="G83"/>
     </row>
     <row r="84" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
@@ -2901,6 +4162,9 @@
       <c r="D84" s="0" t="s">
         <v>223</v>
       </c>
+      <c r="E84"/>
+      <c r="F84"/>
+      <c r="G84"/>
     </row>
     <row r="85" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
@@ -2915,6 +4179,9 @@
       <c r="D85" s="0" t="s">
         <v>225</v>
       </c>
+      <c r="E85"/>
+      <c r="F85"/>
+      <c r="G85"/>
     </row>
     <row r="86" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
@@ -2929,6 +4196,9 @@
       <c r="D86" s="0" t="s">
         <v>228</v>
       </c>
+      <c r="E86"/>
+      <c r="F86"/>
+      <c r="G86"/>
     </row>
     <row r="87" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
@@ -2943,6 +4213,9 @@
       <c r="D87" s="0" t="s">
         <v>229</v>
       </c>
+      <c r="E87"/>
+      <c r="F87"/>
+      <c r="G87"/>
     </row>
     <row r="88" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
@@ -2957,6 +4230,9 @@
       <c r="D88" s="0" t="s">
         <v>232</v>
       </c>
+      <c r="E88"/>
+      <c r="F88"/>
+      <c r="G88"/>
     </row>
     <row r="89" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
@@ -2971,6 +4247,9 @@
       <c r="D89" s="0" t="s">
         <v>236</v>
       </c>
+      <c r="E89"/>
+      <c r="F89"/>
+      <c r="G89"/>
     </row>
     <row r="90" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
@@ -2985,6 +4264,9 @@
       <c r="D90" s="0" t="s">
         <v>238</v>
       </c>
+      <c r="E90"/>
+      <c r="F90"/>
+      <c r="G90"/>
     </row>
     <row r="91" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
@@ -2999,6 +4281,9 @@
       <c r="D91" s="0" t="s">
         <v>240</v>
       </c>
+      <c r="E91"/>
+      <c r="F91"/>
+      <c r="G91"/>
     </row>
     <row r="92" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
@@ -3013,6 +4298,9 @@
       <c r="D92" s="0" t="s">
         <v>241</v>
       </c>
+      <c r="E92"/>
+      <c r="F92"/>
+      <c r="G92"/>
     </row>
     <row r="93" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
@@ -3027,6 +4315,9 @@
       <c r="D93" s="0" t="s">
         <v>245</v>
       </c>
+      <c r="E93"/>
+      <c r="F93"/>
+      <c r="G93"/>
     </row>
     <row r="94" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
@@ -3041,6 +4332,9 @@
       <c r="D94" s="0" t="s">
         <v>248</v>
       </c>
+      <c r="E94"/>
+      <c r="F94"/>
+      <c r="G94"/>
     </row>
     <row r="95" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
@@ -3055,6 +4349,9 @@
       <c r="D95" s="0" t="s">
         <v>251</v>
       </c>
+      <c r="E95"/>
+      <c r="F95"/>
+      <c r="G95"/>
     </row>
     <row r="96" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
@@ -3069,6 +4366,9 @@
       <c r="D96" s="0" t="s">
         <v>254</v>
       </c>
+      <c r="E96"/>
+      <c r="F96"/>
+      <c r="G96"/>
     </row>
     <row r="97" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
@@ -3083,6 +4383,9 @@
       <c r="D97" s="0" t="s">
         <v>256</v>
       </c>
+      <c r="E97"/>
+      <c r="F97"/>
+      <c r="G97"/>
     </row>
     <row r="98" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
@@ -3097,6 +4400,9 @@
       <c r="D98" s="0" t="s">
         <v>258</v>
       </c>
+      <c r="E98"/>
+      <c r="F98"/>
+      <c r="G98"/>
     </row>
     <row r="99" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
@@ -3111,6 +4417,9 @@
       <c r="D99" s="0" t="s">
         <v>262</v>
       </c>
+      <c r="E99"/>
+      <c r="F99"/>
+      <c r="G99"/>
     </row>
     <row r="100" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
@@ -3125,6 +4434,9 @@
       <c r="D100" s="0" t="s">
         <v>266</v>
       </c>
+      <c r="E100"/>
+      <c r="F100"/>
+      <c r="G100"/>
     </row>
     <row r="101" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
@@ -3139,6 +4451,9 @@
       <c r="D101" s="0" t="s">
         <v>268</v>
       </c>
+      <c r="E101"/>
+      <c r="F101"/>
+      <c r="G101"/>
     </row>
     <row r="102" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
@@ -3153,6 +4468,9 @@
       <c r="D102" s="0" t="s">
         <v>270</v>
       </c>
+      <c r="E102"/>
+      <c r="F102"/>
+      <c r="G102"/>
     </row>
     <row r="103" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
@@ -3167,6 +4485,9 @@
       <c r="D103" s="0" t="s">
         <v>272</v>
       </c>
+      <c r="E103"/>
+      <c r="F103"/>
+      <c r="G103"/>
     </row>
     <row r="104" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
@@ -3181,6 +4502,9 @@
       <c r="D104" s="0" t="s">
         <v>275</v>
       </c>
+      <c r="E104"/>
+      <c r="F104"/>
+      <c r="G104"/>
     </row>
     <row r="105" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
@@ -3195,6 +4519,9 @@
       <c r="D105" s="0" t="s">
         <v>277</v>
       </c>
+      <c r="E105"/>
+      <c r="F105"/>
+      <c r="G105"/>
     </row>
     <row r="106" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
@@ -3209,6 +4536,9 @@
       <c r="D106" s="0" t="s">
         <v>277</v>
       </c>
+      <c r="E106"/>
+      <c r="F106"/>
+      <c r="G106"/>
     </row>
     <row r="107" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
@@ -3223,6 +4553,9 @@
       <c r="D107" s="0" t="s">
         <v>278</v>
       </c>
+      <c r="E107"/>
+      <c r="F107"/>
+      <c r="G107"/>
     </row>
     <row r="108" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
@@ -3237,6 +4570,9 @@
       <c r="D108" s="0" t="s">
         <v>278</v>
       </c>
+      <c r="E108"/>
+      <c r="F108"/>
+      <c r="G108"/>
     </row>
     <row r="109" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
@@ -3251,6 +4587,9 @@
       <c r="D109" s="0" t="s">
         <v>279</v>
       </c>
+      <c r="E109"/>
+      <c r="F109"/>
+      <c r="G109"/>
     </row>
     <row r="110" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
@@ -3265,6 +4604,9 @@
       <c r="D110" s="0" t="s">
         <v>280</v>
       </c>
+      <c r="E110"/>
+      <c r="F110"/>
+      <c r="G110"/>
     </row>
     <row r="111" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
@@ -3279,6 +4621,9 @@
       <c r="D111" s="0" t="s">
         <v>283</v>
       </c>
+      <c r="E111"/>
+      <c r="F111"/>
+      <c r="G111"/>
     </row>
     <row r="112" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
@@ -3293,6 +4638,9 @@
       <c r="D112" s="0" t="s">
         <v>283</v>
       </c>
+      <c r="E112"/>
+      <c r="F112"/>
+      <c r="G112"/>
     </row>
     <row r="113" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
@@ -3307,6 +4655,9 @@
       <c r="D113" s="0" t="s">
         <v>279</v>
       </c>
+      <c r="E113"/>
+      <c r="F113"/>
+      <c r="G113"/>
     </row>
     <row r="114" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
@@ -3321,6 +4672,9 @@
       <c r="D114" s="0" t="s">
         <v>286</v>
       </c>
+      <c r="E114"/>
+      <c r="F114"/>
+      <c r="G114"/>
     </row>
     <row r="115" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
@@ -3335,6 +4689,9 @@
       <c r="D115" s="0" t="s">
         <v>286</v>
       </c>
+      <c r="E115"/>
+      <c r="F115"/>
+      <c r="G115"/>
     </row>
     <row r="116" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
@@ -3349,6 +4706,9 @@
       <c r="D116" s="0" t="s">
         <v>288</v>
       </c>
+      <c r="E116"/>
+      <c r="F116"/>
+      <c r="G116"/>
     </row>
     <row r="117" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
@@ -3363,6 +4723,9 @@
       <c r="D117" s="0" t="s">
         <v>291</v>
       </c>
+      <c r="E117"/>
+      <c r="F117"/>
+      <c r="G117"/>
     </row>
     <row r="118" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
@@ -3377,6 +4740,9 @@
       <c r="D118" s="0" t="s">
         <v>293</v>
       </c>
+      <c r="E118"/>
+      <c r="F118"/>
+      <c r="G118"/>
     </row>
     <row r="119" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
@@ -3391,6 +4757,9 @@
       <c r="D119" s="0" t="s">
         <v>296</v>
       </c>
+      <c r="E119"/>
+      <c r="F119"/>
+      <c r="G119"/>
     </row>
     <row r="120" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
@@ -3405,6 +4774,9 @@
       <c r="D120" s="0" t="s">
         <v>298</v>
       </c>
+      <c r="E120"/>
+      <c r="F120"/>
+      <c r="G120"/>
     </row>
     <row r="121" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
@@ -3419,6 +4791,9 @@
       <c r="D121" s="0" t="s">
         <v>298</v>
       </c>
+      <c r="E121"/>
+      <c r="F121"/>
+      <c r="G121"/>
     </row>
     <row r="122" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
@@ -3433,6 +4808,9 @@
       <c r="D122" s="0" t="s">
         <v>298</v>
       </c>
+      <c r="E122"/>
+      <c r="F122"/>
+      <c r="G122"/>
     </row>
     <row r="123" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
@@ -3447,6 +4825,9 @@
       <c r="D123" s="0" t="s">
         <v>298</v>
       </c>
+      <c r="E123"/>
+      <c r="F123"/>
+      <c r="G123"/>
     </row>
     <row r="124" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
@@ -3461,6 +4842,9 @@
       <c r="D124" s="0" t="s">
         <v>298</v>
       </c>
+      <c r="E124"/>
+      <c r="F124"/>
+      <c r="G124"/>
     </row>
     <row r="125" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
@@ -3475,6 +4859,9 @@
       <c r="D125" s="0" t="s">
         <v>301</v>
       </c>
+      <c r="E125"/>
+      <c r="F125"/>
+      <c r="G125"/>
     </row>
     <row r="126" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
@@ -3489,6 +4876,9 @@
       <c r="D126" s="0" t="s">
         <v>301</v>
       </c>
+      <c r="E126"/>
+      <c r="F126"/>
+      <c r="G126"/>
     </row>
     <row r="127" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
@@ -3503,6 +4893,9 @@
       <c r="D127" s="0" t="s">
         <v>301</v>
       </c>
+      <c r="E127"/>
+      <c r="F127"/>
+      <c r="G127"/>
     </row>
     <row r="128" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
@@ -3517,6 +4910,9 @@
       <c r="D128" s="0" t="s">
         <v>301</v>
       </c>
+      <c r="E128"/>
+      <c r="F128"/>
+      <c r="G128"/>
     </row>
     <row r="129" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
@@ -3531,6 +4927,9 @@
       <c r="D129" s="0" t="s">
         <v>301</v>
       </c>
+      <c r="E129"/>
+      <c r="F129"/>
+      <c r="G129"/>
     </row>
     <row r="130" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
@@ -3545,6 +4944,9 @@
       <c r="D130" s="0" t="s">
         <v>301</v>
       </c>
+      <c r="E130"/>
+      <c r="F130"/>
+      <c r="G130"/>
     </row>
     <row r="131" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
@@ -3559,6 +4961,9 @@
       <c r="D131" s="0" t="s">
         <v>301</v>
       </c>
+      <c r="E131"/>
+      <c r="F131"/>
+      <c r="G131"/>
     </row>
     <row r="132" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
@@ -3573,6 +4978,9 @@
       <c r="D132" s="0" t="s">
         <v>301</v>
       </c>
+      <c r="E132"/>
+      <c r="F132"/>
+      <c r="G132"/>
     </row>
     <row r="133" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
@@ -3587,6 +4995,9 @@
       <c r="D133" s="0" t="s">
         <v>301</v>
       </c>
+      <c r="E133"/>
+      <c r="F133"/>
+      <c r="G133"/>
     </row>
     <row r="134" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
@@ -3601,6 +5012,9 @@
       <c r="D134" s="0" t="s">
         <v>305</v>
       </c>
+      <c r="E134"/>
+      <c r="F134"/>
+      <c r="G134"/>
     </row>
     <row r="135" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
@@ -3615,6 +5029,9 @@
       <c r="D135" s="0" t="s">
         <v>305</v>
       </c>
+      <c r="E135"/>
+      <c r="F135"/>
+      <c r="G135"/>
     </row>
     <row r="136" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
@@ -3629,6 +5046,9 @@
       <c r="D136" s="0" t="s">
         <v>305</v>
       </c>
+      <c r="E136"/>
+      <c r="F136"/>
+      <c r="G136"/>
     </row>
     <row r="137" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
@@ -3643,6 +5063,9 @@
       <c r="D137" s="0" t="s">
         <v>305</v>
       </c>
+      <c r="E137"/>
+      <c r="F137"/>
+      <c r="G137"/>
     </row>
     <row r="138" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
@@ -3657,6 +5080,9 @@
       <c r="D138" s="0" t="s">
         <v>305</v>
       </c>
+      <c r="E138"/>
+      <c r="F138"/>
+      <c r="G138"/>
     </row>
     <row r="139" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
@@ -3671,6 +5097,9 @@
       <c r="D139" s="0" t="s">
         <v>305</v>
       </c>
+      <c r="E139"/>
+      <c r="F139"/>
+      <c r="G139"/>
     </row>
     <row r="140" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
@@ -3685,6 +5114,9 @@
       <c r="D140" s="0" t="s">
         <v>305</v>
       </c>
+      <c r="E140"/>
+      <c r="F140"/>
+      <c r="G140"/>
     </row>
     <row r="141" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
@@ -3699,6 +5131,9 @@
       <c r="D141" s="0" t="s">
         <v>305</v>
       </c>
+      <c r="E141"/>
+      <c r="F141"/>
+      <c r="G141"/>
     </row>
     <row r="142" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
@@ -3713,6 +5148,9 @@
       <c r="D142" s="0" t="s">
         <v>305</v>
       </c>
+      <c r="E142"/>
+      <c r="F142"/>
+      <c r="G142"/>
     </row>
     <row r="143" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
@@ -3727,6 +5165,9 @@
       <c r="D143" s="0" t="s">
         <v>307</v>
       </c>
+      <c r="E143"/>
+      <c r="F143"/>
+      <c r="G143"/>
     </row>
     <row r="144" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
@@ -3741,6 +5182,9 @@
       <c r="D144" s="0" t="s">
         <v>307</v>
       </c>
+      <c r="E144"/>
+      <c r="F144"/>
+      <c r="G144"/>
     </row>
     <row r="145" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
@@ -3755,6 +5199,9 @@
       <c r="D145" s="0" t="s">
         <v>307</v>
       </c>
+      <c r="E145"/>
+      <c r="F145"/>
+      <c r="G145"/>
     </row>
     <row r="146" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
@@ -3769,6 +5216,9 @@
       <c r="D146" s="0" t="s">
         <v>307</v>
       </c>
+      <c r="E146"/>
+      <c r="F146"/>
+      <c r="G146"/>
     </row>
     <row r="147" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
@@ -3783,6 +5233,9 @@
       <c r="D147" s="0" t="s">
         <v>307</v>
       </c>
+      <c r="E147"/>
+      <c r="F147"/>
+      <c r="G147"/>
     </row>
     <row r="148" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
@@ -3797,6 +5250,9 @@
       <c r="D148" s="0" t="s">
         <v>307</v>
       </c>
+      <c r="E148"/>
+      <c r="F148"/>
+      <c r="G148"/>
     </row>
     <row r="149" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
@@ -3811,6 +5267,9 @@
       <c r="D149" s="0" t="s">
         <v>309</v>
       </c>
+      <c r="E149"/>
+      <c r="F149"/>
+      <c r="G149"/>
     </row>
     <row r="150" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
@@ -3825,6 +5284,9 @@
       <c r="D150" s="0" t="s">
         <v>310</v>
       </c>
+      <c r="E150"/>
+      <c r="F150"/>
+      <c r="G150"/>
     </row>
     <row r="151" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
@@ -3839,6 +5301,9 @@
       <c r="D151" s="0" t="s">
         <v>311</v>
       </c>
+      <c r="E151"/>
+      <c r="F151"/>
+      <c r="G151"/>
     </row>
     <row r="152" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
@@ -3853,6 +5318,9 @@
       <c r="D152" s="0" t="s">
         <v>312</v>
       </c>
+      <c r="E152"/>
+      <c r="F152"/>
+      <c r="G152"/>
     </row>
     <row r="153" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
@@ -3867,6 +5335,9 @@
       <c r="D153" s="0" t="s">
         <v>313</v>
       </c>
+      <c r="E153"/>
+      <c r="F153"/>
+      <c r="G153"/>
     </row>
     <row r="154" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
@@ -3881,6 +5352,9 @@
       <c r="D154" s="0" t="s">
         <v>314</v>
       </c>
+      <c r="E154"/>
+      <c r="F154"/>
+      <c r="G154"/>
     </row>
     <row r="155" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
@@ -3895,6 +5369,9 @@
       <c r="D155" s="0" t="s">
         <v>315</v>
       </c>
+      <c r="E155"/>
+      <c r="F155"/>
+      <c r="G155"/>
     </row>
     <row r="156" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
@@ -3909,6 +5386,9 @@
       <c r="D156" s="0" t="s">
         <v>316</v>
       </c>
+      <c r="E156"/>
+      <c r="F156"/>
+      <c r="G156"/>
     </row>
     <row r="157" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
@@ -3923,6 +5403,9 @@
       <c r="D157" s="0" t="s">
         <v>317</v>
       </c>
+      <c r="E157"/>
+      <c r="F157"/>
+      <c r="G157"/>
     </row>
     <row r="158" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
@@ -3937,6 +5420,9 @@
       <c r="D158" s="0" t="s">
         <v>319</v>
       </c>
+      <c r="E158"/>
+      <c r="F158"/>
+      <c r="G158"/>
     </row>
     <row r="159" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
@@ -3951,6 +5437,9 @@
       <c r="D159" s="0" t="s">
         <v>319</v>
       </c>
+      <c r="E159"/>
+      <c r="F159"/>
+      <c r="G159"/>
     </row>
     <row r="160" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
@@ -3965,6 +5454,9 @@
       <c r="D160" s="0" t="s">
         <v>319</v>
       </c>
+      <c r="E160"/>
+      <c r="F160"/>
+      <c r="G160"/>
     </row>
     <row r="161" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
@@ -3979,6 +5471,9 @@
       <c r="D161" s="0" t="s">
         <v>319</v>
       </c>
+      <c r="E161"/>
+      <c r="F161"/>
+      <c r="G161"/>
     </row>
     <row r="162" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
@@ -3993,6 +5488,9 @@
       <c r="D162" s="0" t="s">
         <v>319</v>
       </c>
+      <c r="E162"/>
+      <c r="F162"/>
+      <c r="G162"/>
     </row>
     <row r="163" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
@@ -4007,6 +5505,9 @@
       <c r="D163" s="0" t="s">
         <v>319</v>
       </c>
+      <c r="E163"/>
+      <c r="F163"/>
+      <c r="G163"/>
     </row>
     <row r="164" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
@@ -4024,6 +5525,8 @@
       <c r="E164" s="0" t="s">
         <v>324</v>
       </c>
+      <c r="F164"/>
+      <c r="G164"/>
     </row>
     <row r="165" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
@@ -4041,6 +5544,8 @@
       <c r="E165" s="0" t="s">
         <v>324</v>
       </c>
+      <c r="F165"/>
+      <c r="G165"/>
     </row>
     <row r="166" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
@@ -4058,6 +5563,8 @@
       <c r="E166" s="0" t="s">
         <v>329</v>
       </c>
+      <c r="F166"/>
+      <c r="G166"/>
     </row>
     <row r="167" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
@@ -4072,6 +5579,9 @@
       <c r="D167" s="0" t="s">
         <v>330</v>
       </c>
+      <c r="E167"/>
+      <c r="F167"/>
+      <c r="G167"/>
     </row>
     <row r="168" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
@@ -4086,6 +5596,9 @@
       <c r="D168" s="0" t="s">
         <v>331</v>
       </c>
+      <c r="E168"/>
+      <c r="F168"/>
+      <c r="G168"/>
     </row>
     <row r="169" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
@@ -4100,6 +5613,9 @@
       <c r="D169" s="0" t="s">
         <v>332</v>
       </c>
+      <c r="E169"/>
+      <c r="F169"/>
+      <c r="G169"/>
     </row>
     <row r="170" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
@@ -4114,6 +5630,9 @@
       <c r="D170" s="0" t="s">
         <v>333</v>
       </c>
+      <c r="E170"/>
+      <c r="F170"/>
+      <c r="G170"/>
     </row>
     <row r="171" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
@@ -4128,6 +5647,9 @@
       <c r="D171" s="0" t="s">
         <v>334</v>
       </c>
+      <c r="E171"/>
+      <c r="F171"/>
+      <c r="G171"/>
     </row>
     <row r="172" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
@@ -4142,6 +5664,9 @@
       <c r="D172" s="0" t="s">
         <v>338</v>
       </c>
+      <c r="E172"/>
+      <c r="F172"/>
+      <c r="G172"/>
     </row>
     <row r="173" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
@@ -4156,6 +5681,9 @@
       <c r="D173" s="0" t="s">
         <v>340</v>
       </c>
+      <c r="E173"/>
+      <c r="F173"/>
+      <c r="G173"/>
     </row>
     <row r="174" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
@@ -4170,6 +5698,9 @@
       <c r="D174" s="0" t="s">
         <v>340</v>
       </c>
+      <c r="E174"/>
+      <c r="F174"/>
+      <c r="G174"/>
     </row>
     <row r="175" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
@@ -4184,6 +5715,9 @@
       <c r="D175" s="0" t="s">
         <v>340</v>
       </c>
+      <c r="E175"/>
+      <c r="F175"/>
+      <c r="G175"/>
     </row>
     <row r="176" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
@@ -4198,6 +5732,9 @@
       <c r="D176" s="0" t="s">
         <v>345</v>
       </c>
+      <c r="E176"/>
+      <c r="F176"/>
+      <c r="G176"/>
     </row>
     <row r="177" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
@@ -4212,6 +5749,9 @@
       <c r="D177" s="0" t="s">
         <v>349</v>
       </c>
+      <c r="E177"/>
+      <c r="F177"/>
+      <c r="G177"/>
     </row>
     <row r="178" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
@@ -4226,6 +5766,9 @@
       <c r="D178" s="0" t="s">
         <v>353</v>
       </c>
+      <c r="E178"/>
+      <c r="F178"/>
+      <c r="G178"/>
     </row>
     <row r="179" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
@@ -4240,6 +5783,9 @@
       <c r="D179" s="0" t="s">
         <v>356</v>
       </c>
+      <c r="E179"/>
+      <c r="F179"/>
+      <c r="G179"/>
     </row>
     <row r="180" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
@@ -4254,6 +5800,9 @@
       <c r="D180" s="0" t="s">
         <v>359</v>
       </c>
+      <c r="E180"/>
+      <c r="F180"/>
+      <c r="G180"/>
     </row>
     <row r="181" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
@@ -4268,6 +5817,9 @@
       <c r="D181" s="0" t="s">
         <v>362</v>
       </c>
+      <c r="E181"/>
+      <c r="F181"/>
+      <c r="G181"/>
     </row>
     <row r="182" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="s">
@@ -4282,6 +5834,9 @@
       <c r="D182" s="0" t="s">
         <v>365</v>
       </c>
+      <c r="E182"/>
+      <c r="F182"/>
+      <c r="G182"/>
     </row>
     <row r="183" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="0" t="s">
@@ -4296,6 +5851,9 @@
       <c r="D183" s="0" t="s">
         <v>369</v>
       </c>
+      <c r="E183"/>
+      <c r="F183"/>
+      <c r="G183"/>
     </row>
     <row r="184" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="s">
@@ -4310,6 +5868,9 @@
       <c r="D184" s="0" t="s">
         <v>369</v>
       </c>
+      <c r="E184"/>
+      <c r="F184"/>
+      <c r="G184"/>
     </row>
     <row r="185" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="s">
@@ -4324,6 +5885,9 @@
       <c r="D185" s="0" t="s">
         <v>375</v>
       </c>
+      <c r="E185"/>
+      <c r="F185"/>
+      <c r="G185"/>
     </row>
     <row r="186" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="s">
@@ -4338,6 +5902,9 @@
       <c r="D186" s="0" t="s">
         <v>378</v>
       </c>
+      <c r="E186"/>
+      <c r="F186"/>
+      <c r="G186"/>
     </row>
     <row r="187" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="s">
@@ -4352,6 +5919,9 @@
       <c r="D187" s="0" t="s">
         <v>381</v>
       </c>
+      <c r="E187"/>
+      <c r="F187"/>
+      <c r="G187"/>
     </row>
     <row r="188" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="0" t="s">
@@ -4366,6 +5936,9 @@
       <c r="D188" s="0" t="s">
         <v>384</v>
       </c>
+      <c r="E188"/>
+      <c r="F188"/>
+      <c r="G188"/>
     </row>
     <row r="189" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="0" t="s">
@@ -4383,6 +5956,8 @@
       <c r="E189" s="0" t="s">
         <v>388</v>
       </c>
+      <c r="F189"/>
+      <c r="G189"/>
     </row>
     <row r="190" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="0" t="s">
@@ -4400,6 +5975,8 @@
       <c r="E190" s="0" t="s">
         <v>392</v>
       </c>
+      <c r="F190"/>
+      <c r="G190"/>
     </row>
     <row r="191" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="0" t="s">
@@ -4414,6 +5991,9 @@
       <c r="D191" s="0" t="s">
         <v>395</v>
       </c>
+      <c r="E191"/>
+      <c r="F191"/>
+      <c r="G191"/>
     </row>
     <row r="192" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="0" t="s">
@@ -4431,6 +6011,8 @@
       <c r="E192" s="0" t="s">
         <v>399</v>
       </c>
+      <c r="F192"/>
+      <c r="G192"/>
     </row>
     <row r="193" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="0" t="s">
@@ -4448,6 +6030,8 @@
       <c r="E193" s="0" t="s">
         <v>403</v>
       </c>
+      <c r="F193"/>
+      <c r="G193"/>
     </row>
     <row r="194" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="0" t="s">
@@ -4465,6 +6049,8 @@
       <c r="E194" s="0" t="s">
         <v>407</v>
       </c>
+      <c r="F194"/>
+      <c r="G194"/>
     </row>
     <row r="195" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="0" t="s">
@@ -4482,6 +6068,8 @@
       <c r="E195" s="0" t="s">
         <v>411</v>
       </c>
+      <c r="F195"/>
+      <c r="G195"/>
     </row>
     <row r="196" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="0" t="s">
@@ -4496,6 +6084,9 @@
       <c r="D196" s="0" t="s">
         <v>414</v>
       </c>
+      <c r="E196"/>
+      <c r="F196"/>
+      <c r="G196"/>
     </row>
     <row r="197" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="0" t="s">
@@ -4510,6 +6101,9 @@
       <c r="D197" s="0" t="s">
         <v>416</v>
       </c>
+      <c r="E197"/>
+      <c r="F197"/>
+      <c r="G197"/>
     </row>
     <row r="198" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="0" t="s">
@@ -4524,6 +6118,9 @@
       <c r="D198" s="0" t="s">
         <v>418</v>
       </c>
+      <c r="E198"/>
+      <c r="F198"/>
+      <c r="G198"/>
     </row>
     <row r="199" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="0" t="s">
@@ -4538,6 +6135,9 @@
       <c r="D199" s="0" t="s">
         <v>419</v>
       </c>
+      <c r="E199"/>
+      <c r="F199"/>
+      <c r="G199"/>
     </row>
     <row r="200" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="s">
@@ -4552,6 +6152,9 @@
       <c r="D200" s="0" t="s">
         <v>421</v>
       </c>
+      <c r="E200"/>
+      <c r="F200"/>
+      <c r="G200"/>
     </row>
     <row r="201" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="0" t="s">
@@ -4566,6 +6169,9 @@
       <c r="D201" s="0" t="s">
         <v>422</v>
       </c>
+      <c r="E201"/>
+      <c r="F201"/>
+      <c r="G201"/>
     </row>
     <row r="202" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="0" t="s">
@@ -4583,6 +6189,8 @@
       <c r="E202" s="0" t="s">
         <v>426</v>
       </c>
+      <c r="F202"/>
+      <c r="G202"/>
     </row>
     <row r="203" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="0" t="s">
@@ -4597,6 +6205,9 @@
       <c r="D203" s="0" t="s">
         <v>429</v>
       </c>
+      <c r="E203"/>
+      <c r="F203"/>
+      <c r="G203"/>
     </row>
     <row r="204" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="0" t="s">
@@ -4611,6 +6222,9 @@
       <c r="D204" s="0" t="s">
         <v>432</v>
       </c>
+      <c r="E204"/>
+      <c r="F204"/>
+      <c r="G204"/>
     </row>
     <row r="205" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="0" t="s">
@@ -4625,6 +6239,9 @@
       <c r="D205" s="0" t="s">
         <v>435</v>
       </c>
+      <c r="E205"/>
+      <c r="F205"/>
+      <c r="G205"/>
     </row>
     <row r="206" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="0" t="s">
@@ -4639,6 +6256,9 @@
       <c r="D206" s="0" t="s">
         <v>438</v>
       </c>
+      <c r="E206"/>
+      <c r="F206"/>
+      <c r="G206"/>
     </row>
     <row r="207" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="0" t="s">
@@ -4653,6 +6273,9 @@
       <c r="D207" s="0" t="s">
         <v>441</v>
       </c>
+      <c r="E207"/>
+      <c r="F207"/>
+      <c r="G207"/>
     </row>
     <row r="208" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="0" t="s">
@@ -4667,6 +6290,9 @@
       <c r="D208" s="0" t="s">
         <v>444</v>
       </c>
+      <c r="E208"/>
+      <c r="F208"/>
+      <c r="G208"/>
     </row>
     <row r="209" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="0" t="s">
@@ -4681,6 +6307,9 @@
       <c r="D209" s="0" t="s">
         <v>445</v>
       </c>
+      <c r="E209"/>
+      <c r="F209"/>
+      <c r="G209"/>
     </row>
     <row r="210" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="0" t="s">
@@ -4695,6 +6324,9 @@
       <c r="D210" s="0" t="s">
         <v>446</v>
       </c>
+      <c r="E210"/>
+      <c r="F210"/>
+      <c r="G210"/>
     </row>
     <row r="211" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="0" t="s">
@@ -4709,6 +6341,9 @@
       <c r="D211" s="0" t="s">
         <v>447</v>
       </c>
+      <c r="E211"/>
+      <c r="F211"/>
+      <c r="G211"/>
     </row>
     <row r="212" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="0" t="s">
@@ -4723,6 +6358,9 @@
       <c r="D212" s="0" t="s">
         <v>449</v>
       </c>
+      <c r="E212"/>
+      <c r="F212"/>
+      <c r="G212"/>
     </row>
     <row r="213" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="0" t="s">
@@ -4737,6 +6375,9 @@
       <c r="D213" s="0" t="s">
         <v>452</v>
       </c>
+      <c r="E213"/>
+      <c r="F213"/>
+      <c r="G213"/>
     </row>
     <row r="214" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="0" t="s">
@@ -4754,6 +6395,8 @@
       <c r="E214" s="0" t="s">
         <v>456</v>
       </c>
+      <c r="F214"/>
+      <c r="G214"/>
     </row>
     <row r="215" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="0" t="s">
@@ -4771,6 +6414,8 @@
       <c r="E215" s="0" t="s">
         <v>459</v>
       </c>
+      <c r="F215"/>
+      <c r="G215"/>
     </row>
     <row r="216" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="0" t="s">
@@ -4785,6 +6430,9 @@
       <c r="D216" s="0" t="s">
         <v>463</v>
       </c>
+      <c r="E216"/>
+      <c r="F216"/>
+      <c r="G216"/>
     </row>
     <row r="217" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="0" t="s">
@@ -4799,6 +6447,9 @@
       <c r="D217" s="0" t="s">
         <v>466</v>
       </c>
+      <c r="E217"/>
+      <c r="F217"/>
+      <c r="G217"/>
     </row>
     <row r="218" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="0" t="s">
@@ -4813,6 +6464,9 @@
       <c r="D218" s="0" t="s">
         <v>469</v>
       </c>
+      <c r="E218"/>
+      <c r="F218"/>
+      <c r="G218"/>
     </row>
     <row r="219" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="0" t="s">
@@ -4830,6 +6484,8 @@
       <c r="E219" s="0" t="s">
         <v>473</v>
       </c>
+      <c r="F219"/>
+      <c r="G219"/>
     </row>
     <row r="220" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="0" t="s">
@@ -4847,6 +6503,8 @@
       <c r="E220" s="0" t="s">
         <v>477</v>
       </c>
+      <c r="F220"/>
+      <c r="G220"/>
     </row>
     <row r="221" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="0" t="s">
@@ -4864,6 +6522,8 @@
       <c r="E221" s="0" t="s">
         <v>481</v>
       </c>
+      <c r="F221"/>
+      <c r="G221"/>
     </row>
     <row r="222" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="0" t="s">
@@ -4881,6 +6541,8 @@
       <c r="E222" s="0" t="s">
         <v>485</v>
       </c>
+      <c r="F222"/>
+      <c r="G222"/>
     </row>
     <row r="223" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="0" t="s">
@@ -4898,6 +6560,8 @@
       <c r="E223" s="0" t="s">
         <v>489</v>
       </c>
+      <c r="F223"/>
+      <c r="G223"/>
     </row>
     <row r="224" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="0" t="s">
@@ -4915,6 +6579,8 @@
       <c r="E224" s="0" t="s">
         <v>493</v>
       </c>
+      <c r="F224"/>
+      <c r="G224"/>
     </row>
     <row r="225" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="0" t="s">
@@ -4932,6 +6598,8 @@
       <c r="E225" s="0" t="s">
         <v>497</v>
       </c>
+      <c r="F225"/>
+      <c r="G225"/>
     </row>
     <row r="226" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="0" t="s">
@@ -4946,6 +6614,9 @@
       <c r="D226" s="0" t="s">
         <v>501</v>
       </c>
+      <c r="E226"/>
+      <c r="F226"/>
+      <c r="G226"/>
     </row>
     <row r="227" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="0" t="s">
@@ -4960,6 +6631,9 @@
       <c r="D227" s="0" t="s">
         <v>504</v>
       </c>
+      <c r="E227"/>
+      <c r="F227"/>
+      <c r="G227"/>
     </row>
     <row r="228" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="0" t="s">
@@ -4974,6 +6648,9 @@
       <c r="D228" s="0" t="s">
         <v>507</v>
       </c>
+      <c r="E228"/>
+      <c r="F228"/>
+      <c r="G228"/>
     </row>
     <row r="229" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="0" t="s">
@@ -4988,6 +6665,9 @@
       <c r="D229" s="0" t="s">
         <v>509</v>
       </c>
+      <c r="E229"/>
+      <c r="F229"/>
+      <c r="G229"/>
     </row>
     <row r="230" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="0" t="s">
@@ -5002,6 +6682,9 @@
       <c r="D230" s="0" t="s">
         <v>511</v>
       </c>
+      <c r="E230"/>
+      <c r="F230"/>
+      <c r="G230"/>
     </row>
     <row r="231" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="0" t="s">
@@ -5016,6 +6699,9 @@
       <c r="D231" s="0" t="s">
         <v>513</v>
       </c>
+      <c r="E231"/>
+      <c r="F231"/>
+      <c r="G231"/>
     </row>
     <row r="232" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="0" t="s">
@@ -5030,8 +6716,19 @@
       <c r="D232" s="0" t="s">
         <v>515</v>
       </c>
-    </row>
-    <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="E232"/>
+      <c r="F232"/>
+      <c r="G232"/>
+    </row>
+    <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A233"/>
+      <c r="B233"/>
+      <c r="C233"/>
+      <c r="D233"/>
+      <c r="E233"/>
+      <c r="F233"/>
+      <c r="G233"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>